<commit_message>
experiments data used for testing
</commit_message>
<xml_diff>
--- a/results/network.xlsx
+++ b/results/network.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
   <si>
     <t>d</t>
   </si>
@@ -114,31 +114,7 @@
     <t>Config 5</t>
   </si>
   <si>
-    <t>Headset A - Fog - Original</t>
-  </si>
-  <si>
     <t>Theoretical</t>
-  </si>
-  <si>
-    <t>Headset A - Fog - Addressing</t>
-  </si>
-  <si>
-    <t>Headset B - Fog - Original</t>
-  </si>
-  <si>
-    <t>Headset A - Cloud - Original</t>
-  </si>
-  <si>
-    <t>Headset B - Cloud - Original</t>
-  </si>
-  <si>
-    <t>Headset B - Fog - Addressing</t>
-  </si>
-  <si>
-    <t>Headset A - Cloud - Addressing</t>
-  </si>
-  <si>
-    <t>Headset B - Cloud - Addressing</t>
   </si>
   <si>
     <t>Addressing</t>
@@ -148,6 +124,51 @@
   </si>
   <si>
     <t>Experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Конф 1</t>
+  </si>
+  <si>
+    <t>Тип A - Туман. - Адрес.</t>
+  </si>
+  <si>
+    <t>Тип A - Туман. - Оригін.</t>
+  </si>
+  <si>
+    <t>Тип Б - Туман. - Оригін.</t>
+  </si>
+  <si>
+    <t>Тип Б - Туман. - Адрес.</t>
+  </si>
+  <si>
+    <t>Тип А - Хмар. - Оригін.</t>
+  </si>
+  <si>
+    <t>Тип А - Хмар. - Адрес.</t>
+  </si>
+  <si>
+    <t>Тип Б - Хмар. - Оригін.</t>
+  </si>
+  <si>
+    <t>Тип Б - Хмар. - Адрес.</t>
+  </si>
+  <si>
+    <t>Конфіг. 1</t>
+  </si>
+  <si>
+    <t>Конфіг. 2</t>
+  </si>
+  <si>
+    <t>Конфіг. 3</t>
+  </si>
+  <si>
+    <t>Конфіг. 4</t>
+  </si>
+  <si>
+    <t>Конфіг. 5</t>
   </si>
 </sst>
 </file>
@@ -265,19 +286,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -327,19 +348,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -389,19 +410,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -451,19 +472,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -513,19 +534,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -575,19 +596,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -637,19 +658,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -699,19 +720,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -741,11 +762,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="49820032"/>
-        <c:axId val="49821952"/>
+        <c:axId val="130668800"/>
+        <c:axId val="130499328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49820032"/>
+        <c:axId val="130668800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,14 +790,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49821952"/>
+        <c:crossAx val="130499328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49821952"/>
+        <c:axId val="130499328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +824,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49820032"/>
+        <c:crossAx val="130668800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -817,7 +838,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -826,7 +847,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
-  <c:style val="5"/>
+  <c:style val="1"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -834,39 +855,23 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Addressing Average Network Usage</a:t>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Addressing Average Network Usage(theoretical vs experimental)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
-              <a:t>(theoretical vs experimental)</a:t>
-            </a:r>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="ru-RU">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -897,19 +902,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -959,19 +964,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1021,19 +1026,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1083,19 +1088,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1145,19 +1150,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1207,19 +1212,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1269,19 +1274,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1331,19 +1336,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1373,11 +1378,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="47472640"/>
-        <c:axId val="47474560"/>
+        <c:axId val="131156224"/>
+        <c:axId val="131170688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="47472640"/>
+        <c:axId val="131156224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1401,14 +1406,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47474560"/>
+        <c:crossAx val="131170688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47474560"/>
+        <c:axId val="131170688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500"/>
@@ -1436,7 +1441,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47472640"/>
+        <c:crossAx val="131156224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1450,7 +1455,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1459,44 +1464,21 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
-  <c:style val="5"/>
+  <c:style val="1"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Theoretical</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Network Usage (origina</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>l vs </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>addressing)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13207082716145627"/>
+          <c:y val="3.394092341110589E-2"/>
+          <c:w val="0.8572651438372183"/>
+          <c:h val="0.83271803524559451"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1509,7 +1491,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Fog - Original</c:v>
+                  <c:v>Тип A - Туман. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1520,19 +1502,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1571,7 +1553,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Fog - Addressing</c:v>
+                  <c:v>Тип A - Туман. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1582,19 +1564,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1633,7 +1615,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Fog - Original</c:v>
+                  <c:v>Тип Б - Туман. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1644,19 +1626,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1695,7 +1677,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Fog - Addressing</c:v>
+                  <c:v>Тип Б - Туман. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1706,19 +1688,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1757,7 +1739,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Cloud - Original</c:v>
+                  <c:v>Тип А - Хмар. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1768,19 +1750,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1819,7 +1801,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Cloud - Addressing</c:v>
+                  <c:v>Тип А - Хмар. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1830,19 +1812,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1881,7 +1863,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Cloud - Original</c:v>
+                  <c:v>Тип Б - Хмар. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1892,19 +1874,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1943,7 +1925,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Cloud - Addressing</c:v>
+                  <c:v>Тип Б - Хмар. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1954,19 +1936,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1996,42 +1978,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134427392"/>
-        <c:axId val="134430080"/>
+        <c:axId val="131296640"/>
+        <c:axId val="131306624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134427392"/>
+        <c:axId val="131296640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Physical Topology Configurations</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134430080"/>
+        <c:crossAx val="131306624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134430080"/>
+        <c:axId val="131306624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500"/>
@@ -2048,8 +2012,8 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Network Usage (in KyloBytes)</a:t>
+                  <a:rPr lang="uk-UA"/>
+                  <a:t>Навантаження мережі (кБайт)</a:t>
                 </a:r>
                 <a:endParaRPr lang="ru-RU"/>
               </a:p>
@@ -2059,21 +2023,43 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134427392"/>
+        <c:crossAx val="131296640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13407129492476808"/>
+          <c:y val="3.5968280451239253E-2"/>
+          <c:w val="0.38082579714664394"/>
+          <c:h val="0.6629032620922386"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2082,44 +2068,21 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
-  <c:style val="5"/>
+  <c:style val="1"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Theoretical</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Network Usage (origina</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>l vs </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>addressing)</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15164500248725776"/>
+          <c:y val="5.247536949021088E-2"/>
+          <c:w val="0.83607821028802498"/>
+          <c:h val="0.81763802408101482"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2132,7 +2095,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Fog - Original</c:v>
+                  <c:v>Тип A - Туман. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2143,19 +2106,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2194,7 +2157,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Fog - Addressing</c:v>
+                  <c:v>Тип A - Туман. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2205,19 +2168,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2256,7 +2219,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Fog - Original</c:v>
+                  <c:v>Тип Б - Туман. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2267,19 +2230,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2318,7 +2281,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Fog - Addressing</c:v>
+                  <c:v>Тип Б - Туман. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2329,19 +2292,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2380,7 +2343,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Cloud - Original</c:v>
+                  <c:v>Тип А - Хмар. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2391,19 +2354,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2442,7 +2405,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset A - Cloud - Addressing</c:v>
+                  <c:v>Тип А - Хмар. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2453,19 +2416,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2504,7 +2467,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Cloud - Original</c:v>
+                  <c:v>Тип Б - Хмар. - Оригін.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2515,19 +2478,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2566,7 +2529,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Headset B - Cloud - Addressing</c:v>
+                  <c:v>Тип Б - Хмар. - Адрес.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2577,19 +2540,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Config 1</c:v>
+                  <c:v>Конфіг. 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Config 2</c:v>
+                  <c:v>Конфіг. 2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Config 3</c:v>
+                  <c:v>Конфіг. 3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Config 4</c:v>
+                  <c:v>Конфіг. 4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Config 5</c:v>
+                  <c:v>Конфіг. 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2619,42 +2582,37 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="134530944"/>
-        <c:axId val="125771776"/>
+        <c:axId val="131207936"/>
+        <c:axId val="131209856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134530944"/>
+        <c:axId val="131207936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Physical Topology Configurations</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125771776"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="131209856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125771776"/>
+        <c:axId val="131209856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500"/>
@@ -2668,13 +2626,22 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1100">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Network Usage (in KyloBytes)</a:t>
+                  <a:rPr lang="uk-UA" sz="1100">
+                    <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Навантаження мережі (кБайт)</a:t>
                 </a:r>
-                <a:endParaRPr lang="ru-RU"/>
+                <a:endParaRPr lang="ru-RU" sz="1100">
+                  <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2682,21 +2649,56 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134530944"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100">
+                <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="131207936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14946534108298273"/>
+          <c:y val="4.9420676416526463E-2"/>
+          <c:w val="0.41102567627214098"/>
+          <c:h val="0.63647775429445264"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100">
+              <a:latin typeface="Times New Roman" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2766,16 +2768,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>177801</xdr:rowOff>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>549565</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>122381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>469053</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>48004</xdr:rowOff>
+      <xdr:colOff>988292</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>175490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2796,16 +2798,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>643467</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>534170</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>5388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>367453</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>39536</xdr:rowOff>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3114,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BL49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BB15" sqref="BB15"/>
+    <sheetView tabSelected="1" topLeftCell="AV10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BG26" sqref="BG26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3129,7 +3131,7 @@
     <col min="14" max="14" width="8.88671875" customWidth="1"/>
     <col min="17" max="17" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.88671875" customWidth="1"/>
     <col min="22" max="22" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -3153,7 +3155,7 @@
     <col min="63" max="64" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="57.6">
+    <row r="1" spans="1:64" ht="43.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -3220,52 +3222,52 @@
         <v>26</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="AV1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AW1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="BE1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="BH1" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:64">
@@ -3315,7 +3317,7 @@
         <v>18</v>
       </c>
       <c r="T2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="U2">
         <f>$Q9</f>
@@ -3384,8 +3386,11 @@
         <f>$R39</f>
         <v>77.273800000000008</v>
       </c>
+      <c r="AQ2" t="s">
+        <v>36</v>
+      </c>
       <c r="AR2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="AS2">
         <f>$Q9</f>
@@ -3508,7 +3513,7 @@
         <v>8.8003999999999998</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U6" si="0">$Q10</f>
@@ -3701,7 +3706,7 @@
         <v>16.630700000000001</v>
       </c>
       <c r="T4" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
@@ -3894,7 +3899,7 @@
         <v>32.244300000000003</v>
       </c>
       <c r="T5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
@@ -4087,7 +4092,7 @@
         <v>63.567800000000005</v>
       </c>
       <c r="T6" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
@@ -4280,7 +4285,7 @@
         <v>126.18989999999999</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -4291,7 +4296,7 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AF7" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -4302,7 +4307,7 @@
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
       <c r="AS7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AT7" s="3"/>
       <c r="AU7" s="3"/>
@@ -4312,7 +4317,7 @@
       <c r="AY7" s="3"/>
       <c r="AZ7" s="3"/>
       <c r="BD7" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="BE7" s="3"/>
       <c r="BF7" s="3"/>

</xml_diff>